<commit_message>
Subindo arquivo py e tabela atualizada.
</commit_message>
<xml_diff>
--- a/Planilha de testes.xlsx
+++ b/Planilha de testes.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Calculo de carga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luiz Venturini\Documents\repositorio venturini\calculo_de_carga\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1DDE28-0E37-428F-A8BA-EC1C19FE6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>Minimizar ou maximar</t>
   </si>
@@ -356,12 +356,69 @@
   </si>
   <si>
     <t>Peso desejado da liga desejada, em kilograma</t>
+  </si>
+  <si>
+    <t>c_min</t>
+  </si>
+  <si>
+    <t>c_max</t>
+  </si>
+  <si>
+    <t>mn_min</t>
+  </si>
+  <si>
+    <t>mn_max</t>
+  </si>
+  <si>
+    <t>si_min</t>
+  </si>
+  <si>
+    <t>si_max</t>
+  </si>
+  <si>
+    <t>cr_min</t>
+  </si>
+  <si>
+    <t>cr_max</t>
+  </si>
+  <si>
+    <t>ni_min</t>
+  </si>
+  <si>
+    <t>ni_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lista de materiais com Estreitamento_ CQ </t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>cr</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>Material Objetivo</t>
+  </si>
+  <si>
+    <t>A_</t>
+  </si>
+  <si>
+    <t>b_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -539,7 +596,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -821,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,11 +1300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,164 +2176,116 @@
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="S15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="U15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="V15" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="W15" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="X15" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y15" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="D15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
+      <c r="Y15" s="14"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>300</v>
+        <v>1010</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E16">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16">
-        <v>10</v>
+        <v>0.6</v>
       </c>
       <c r="J16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>15</v>
+        <v>0.5</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16">
-        <v>5</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2281,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2290,60 +2306,36 @@
         <v>10</v>
       </c>
       <c r="J17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K17">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>20</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17">
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -2355,69 +2347,45 @@
         <v>0</v>
       </c>
       <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
+      </c>
+      <c r="J18">
         <v>20</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
+      <c r="K18">
+        <v>25</v>
+      </c>
+      <c r="L18">
+        <v>10</v>
+      </c>
+      <c r="M18">
         <v>20</v>
       </c>
-      <c r="J18">
-        <v>10</v>
-      </c>
-      <c r="K18">
-        <v>15</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>0</v>
-      </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
-      <c r="X18">
-        <v>0</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -2429,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2438,146 +2406,98 @@
         <v>20</v>
       </c>
       <c r="J19">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K19">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L19">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>20</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19">
-        <v>0</v>
-      </c>
-      <c r="X19">
-        <v>0</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>57</v>
+      <c r="B20">
+        <v>550</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
       <c r="D20">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>99</v>
+        <v>0.1</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20">
-        <v>0</v>
-      </c>
-      <c r="X20">
-        <v>0</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F21">
-        <v>99.5</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2597,49 +2517,25 @@
       <c r="M21">
         <v>0</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -2648,16 +2544,16 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>99.5</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -2671,49 +2567,25 @@
       <c r="M22">
         <v>0</v>
       </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -2728,16 +2600,16 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="J23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="K23">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2745,118 +2617,965 @@
       <c r="M23">
         <v>0</v>
       </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
-        <v>0</v>
-      </c>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>32</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>50</v>
+      </c>
+      <c r="K24">
+        <v>75</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>61</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>64</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>99.5</v>
       </c>
-      <c r="M24">
+      <c r="M25">
         <v>100</v>
       </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-      <c r="V24">
-        <v>0</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>0</v>
-      </c>
-      <c r="Y24">
-        <v>0</v>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>1010</v>
+      </c>
+      <c r="D27">
+        <v>300</v>
+      </c>
+      <c r="E27">
+        <v>350</v>
+      </c>
+      <c r="F27">
+        <v>500</v>
+      </c>
+      <c r="G27">
+        <v>550</v>
+      </c>
+      <c r="H27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" t="s">
+        <v>59</v>
+      </c>
+      <c r="K27" t="s">
+        <v>60</v>
+      </c>
+      <c r="L27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>16</v>
+      </c>
+      <c r="K28">
+        <v>32</v>
+      </c>
+      <c r="L28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29">
+        <v>0.08</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>97</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="N29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30">
+        <v>0.13</v>
+      </c>
+      <c r="D30">
+        <v>0.1</v>
+      </c>
+      <c r="E30">
+        <v>0.1</v>
+      </c>
+      <c r="F30">
+        <v>0.1</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+      <c r="H30">
+        <v>99</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="N30" s="16">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>99.5</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="N31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B32" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+      <c r="G32">
+        <v>10</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>100</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="N32" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>50</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="N33" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34">
+        <v>0.6</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <v>20</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>70</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="N34" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>20</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>50</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="N35" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>25</v>
+      </c>
+      <c r="F36">
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <v>25</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>75</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="N36" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>99.5</v>
+      </c>
+      <c r="N37" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>20</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>100</v>
+      </c>
+      <c r="N38" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
+        <f>B27</f>
+        <v>material</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:L42" si="0">C27</f>
+        <v>1010</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>550</v>
+      </c>
+      <c r="H42" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="0"/>
+        <v>MN</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="0"/>
+        <v>SI</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>CR</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="0"/>
+        <v>NI</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43">
+        <f>C28</f>
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:L43" si="1">D28</f>
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <f>C29+(C30-C29)*$B$40</f>
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ref="D44:L44" si="2">D29+(D30-D29)*$B$40</f>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="2"/>
+        <v>97.8</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <f>N30</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45">
+        <f>C31+(C32-C31)*$B$40</f>
+        <v>0.4</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45:L45" si="3">D31+(D32-D31)*$B$40</f>
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>99.7</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f>N32</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46">
+        <f>C33+(C34-C33)*$B$40</f>
+        <v>0.24</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ref="D46:L46" si="4">D33+(D34-D33)*$B$40</f>
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <f>N34</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47">
+        <f>C35+(C36-C35)*$B$40</f>
+        <v>0.2</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ref="D47:L47" si="5">D35+(D36-D35)*$B$40</f>
+        <v>12</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f>N36</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48">
+        <f>C37+(C38-C37)*$B$40</f>
+        <v>0.2</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:L48" si="6">D37+(D38-D37)*$B$40</f>
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>99.7</v>
+      </c>
+      <c r="N48">
+        <f>N38</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="str">
+        <f>"["&amp;C43&amp;","&amp;D43&amp;","&amp;E43&amp;","&amp;F43&amp;","&amp;G43&amp;","&amp;H43&amp;","&amp;I43&amp;","&amp;J43&amp;","&amp;K43&amp;","&amp;L43&amp;"]"</f>
+        <v>[1,1,2,3,4,4,8,16,32,64]</v>
+      </c>
+      <c r="E52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="str">
+        <f>"["&amp;C44&amp;","&amp;D44&amp;","&amp;E44&amp;","&amp;F44&amp;","&amp;G44&amp;","&amp;H44&amp;","&amp;I44&amp;","&amp;J44&amp;","&amp;K44&amp;","&amp;L44&amp;"]"</f>
+        <v>[0.1,0.04,0.04,0.04,0.04,97.8,0,0,0,0]</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C54" t="str">
+        <f t="shared" ref="C54:C57" si="7">"["&amp;C45&amp;","&amp;D45&amp;","&amp;E45&amp;","&amp;F45&amp;","&amp;G45&amp;","&amp;H45&amp;","&amp;I45&amp;","&amp;J45&amp;","&amp;K45&amp;","&amp;L45&amp;"]"</f>
+        <v>[0.4,8,4,8,4,0,99.7,0,0,0]</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C55" t="str">
+        <f t="shared" si="7"/>
+        <v>[0.24,4,4,8,8,0,0,58,0,0]</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C56" t="str">
+        <f t="shared" si="7"/>
+        <v>[0.2,12,22,12,22,0,0,0,60,0]</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C57" t="str">
+        <f t="shared" si="7"/>
+        <v>[0.2,2,14,2,14,0,0,0,0,99.7]</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="str">
+        <f>"["&amp;N44&amp;","&amp;N45&amp;","&amp;N46&amp;","&amp;N47&amp;","&amp;N48&amp;"]"</f>
+        <v>[0.12,5,5,18,5]</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>